<commit_message>
finished apparatus, worked on formatting
</commit_message>
<xml_diff>
--- a/collation.xlsx
+++ b/collation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAFC466-4832-4980-A3AB-3684BB8CF960}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7D70CE-E52F-4735-AC60-F1B692EA7742}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,21 +51,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{E6066AF5-5F4C-4311-886B-5278F76EC736}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Author:
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{387460AB-227C-4B27-AF62-0A0A772FDFAD}">
       <text>
         <r>
@@ -528,7 +513,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-note,] ~</t>
+note,]  ~</t>
         </r>
       </text>
     </comment>
@@ -675,22 +660,6 @@
   </si>
   <si>
     <t>so conceived and so dedicated, can long</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">endure. We are met on a great </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>battle-field</t>
-    </r>
   </si>
   <si>
     <t>of that war. We have come to dedicate a</t>
@@ -1057,6 +1026,22 @@
   </si>
   <si>
     <t>place for those who here gave their lives</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">endure. We are met on a great </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>battle_field</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1110,7 +1095,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,12 +1112,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1421,11 +1410,14 @@
   <dimension ref="A1:AS7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD3" sqref="AD3"/>
+      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="42" width="14.7109375" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1437,64 +1429,64 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="3">
         <v>6</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="3">
         <v>7</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="3">
         <v>8</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="3">
         <v>9</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="3">
         <v>10</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="3">
         <v>11</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="3">
         <v>12</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="3">
         <v>13</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="3">
         <v>14</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="3">
         <v>15</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="3">
         <v>16</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:45" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1502,136 +1494,136 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:45" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -1639,80 +1631,96 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="5"/>
+      <c r="U3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AI3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP3" s="5"/>
+      <c r="AR3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AJ3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:45" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1725,79 +1733,97 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="5"/>
+      <c r="X4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AO4" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="AP4" s="5"/>
       <c r="AR4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS4" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:45" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -1805,52 +1831,79 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB5" s="1" t="s">
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AJ5" s="1" t="s">
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AP5" s="5"/>
+      <c r="AR5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AS5" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="AS5" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:45" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1858,127 +1911,172 @@
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
       <c r="AR6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS6" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="AS6" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:45" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="X7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y7" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Z7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="AA7" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AB7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AA7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AE7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AD7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="AJ7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AL7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AM7" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="AM7" s="1" t="s">
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="AO7" s="1" t="s">
+      <c r="AP7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="AP7" s="1" t="s">
+      <c r="AQ7" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AQ7" s="1" t="s">
+      <c r="AR7" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="AR7" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>